<commit_message>
HW2 Grade and Comments
</commit_message>
<xml_diff>
--- a/HW_2_2_2.xlsx
+++ b/HW_2_2_2.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew/Desktop/GMU/GMU MASTER/PHYS 513/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weigel/git/phys513/jackson/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3F3E44-7A89-8B41-8C7B-0334D62A75B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="3680" yWindow="4320" windowWidth="47260" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -180,12 +189,15 @@
   </si>
   <si>
     <t>Is the reason why my analytical solution is different due to me not summing enough integers. I assumed that as I went out past the first 10 integers, the contributions would become less impactful, but maybe I am not going out far enough. I may not be coding the equation right either</t>
+  </si>
+  <si>
+    <t>General idea is correct. See my solutions when I post them.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -230,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +252,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -349,6 +367,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -358,18 +382,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,6 +398,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -646,11 +668,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,10 +681,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="12"/>
       <c r="M1" t="s">
         <v>26</v>
       </c>
@@ -716,10 +738,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="12"/>
       <c r="K2" t="s">
         <v>20</v>
       </c>
@@ -795,10 +817,10 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="13">
         <v>44081</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="13"/>
       <c r="L3">
         <v>3</v>
       </c>
@@ -871,10 +893,10 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="12"/>
       <c r="L4">
         <v>5</v>
       </c>
@@ -1013,10 +1035,10 @@
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="12"/>
       <c r="L6">
         <v>9</v>
       </c>
@@ -1092,12 +1114,12 @@
       <c r="B7">
         <v>100</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
       <c r="L7">
         <v>11</v>
       </c>
@@ -1173,10 +1195,10 @@
       <c r="B8">
         <v>80</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
       <c r="L8">
         <v>13</v>
       </c>
@@ -1252,10 +1274,10 @@
       <c r="B9">
         <v>20</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
       <c r="L9">
         <v>15</v>
       </c>
@@ -1331,10 +1353,10 @@
       <c r="B10">
         <v>60</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
       <c r="L10">
         <v>17</v>
       </c>
@@ -2116,14 +2138,14 @@
       <c r="B20">
         <v>75.2</v>
       </c>
-      <c r="N20" s="12" t="s">
+      <c r="N20" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="12"/>
-      <c r="S20" s="12"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -2132,12 +2154,12 @@
       <c r="B21">
         <v>60.5</v>
       </c>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="12"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -2146,12 +2168,12 @@
       <c r="B22">
         <v>65.400000000000006</v>
       </c>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="12"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -2166,14 +2188,14 @@
         <v>18</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -2184,17 +2206,26 @@
         <v>#VALUE!</v>
       </c>
     </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J27" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+    </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16" t="s">
+      <c r="C28" s="12"/>
+      <c r="D28" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
@@ -2203,19 +2234,19 @@
       <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="I29" s="14" t="s">
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -2231,13 +2262,13 @@
         <f>SUM(M$18,R$18,W$18,AB$18)</f>
         <v>77.986627653439228</v>
       </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -2253,13 +2284,13 @@
         <f t="shared" ref="E31:G33" si="24">SUM(N$18,S$18,X$18,AC$18)</f>
         <v>62.23652494532859</v>
       </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -2275,13 +2306,13 @@
         <f t="shared" si="24"/>
         <v>67.593065286483125</v>
       </c>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
@@ -2297,75 +2328,70 @@
         <f t="shared" si="24"/>
         <v>46.592928342335618</v>
       </c>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="N20:S22"/>
     <mergeCell ref="D7:G10"/>
     <mergeCell ref="I29:O39"/>
@@ -2373,6 +2399,11 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="D28:G29"/>
     <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>